<commit_message>
First version of the UI It has the 70% completed of the total. No major logic coded at the moment, just the buttons to change from one panel to another.
</commit_message>
<xml_diff>
--- a/Assets/Data/DataTable.xlsx
+++ b/Assets/Data/DataTable.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{1322B3DC-77D2-4766-BD39-C04486B7D624}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{448AB268-D732-44BF-9E65-64DDCE2125ED}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ImagesPool" sheetId="3" r:id="rId1"/>
+    <sheet name="Images" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,14 +23,17 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{F7732793-CF5D-4AB9-A66F-060F6A62E9A5}" name="file" type="4" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="file" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\Personal Projects\DataManagerTest\Assets\file.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" xr16:uid="{B0190245-DFF2-4F66-BE61-E6BF3DEC184F}" name="images" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\images.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>Text</t>
   </si>
@@ -48,19 +53,55 @@
     <t>Feña</t>
   </si>
   <si>
-    <t>Suma</t>
-  </si>
-  <si>
-    <t>Promedio</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Recuento</t>
-  </si>
-  <si>
     <t>WenaWena</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PATH</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>td02</t>
+  </si>
+  <si>
+    <t>Blegh</t>
+  </si>
+  <si>
+    <t>Dani</t>
+  </si>
+  <si>
+    <t>Ble</t>
+  </si>
+  <si>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>This is a Bleg</t>
+  </si>
+  <si>
+    <t>This is a Dani</t>
   </si>
 </sst>
 </file>
@@ -103,15 +144,125 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -248,25 +399,86 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema2">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="TextureDataList">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" name="textures" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="TextureData" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:attribute name="id" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="path" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="description" form="unqualified" type="xsd:string"/>
+                    </xsd:complexType>
+                  </xsd:element>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="1" Name="DataTable" RootElement="DataContainer" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="2" Name="TextureDataList_Map" RootElement="TextureDataList" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{388CFA02-1E4E-4B7C-931A-CF3F7687FB0C}" name="Tabla1" displayName="Tabla1" ref="A1:C13" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78A2D084-C518-4315-865E-394057B931C4}" name="Tabla3" displayName="Tabla3" ref="A1:D3" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:D3" xr:uid="{B7105AD6-33EC-435A-A5D1-4F603599336D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0D8D427B-0B9C-44B0-8BCF-7D1DCDFD7373}" uniqueName="id" name="id">
+      <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@id" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{5D10CCD0-71D5-4E31-B900-78CF3B764038}" uniqueName="path" name="path">
+      <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@path" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{6605BEF8-72C9-4692-A87D-8E60862909DF}" uniqueName="name" name="name">
+      <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{204972EE-CF51-4A6E-92C3-45949F7D10AC}" uniqueName="description" name="description">
+      <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@description" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{388CFA02-1E4E-4B7C-931A-CF3F7687FB0C}" name="Tabla1" displayName="Tabla1" ref="A1:C13" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" connectionId="1">
   <autoFilter ref="A1:C13" xr:uid="{02178007-BAB8-4248-9AC0-218326DA414F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{36992CAA-9EDF-435B-A9A8-82F8A6B3C6F5}" uniqueName="Text" name="Text" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{36992CAA-9EDF-435B-A9A8-82F8A6B3C6F5}" uniqueName="Text" name="Text" dataDxfId="8">
       <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/@Text" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{597E18E7-F5C4-42C6-8840-9F56CAFAC4C6}" uniqueName="Number" name="Number" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{597E18E7-F5C4-42C6-8840-9F56CAFAC4C6}" uniqueName="Number" name="Number" dataDxfId="7">
       <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/@Number" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DDC28D44-C5CD-4E4C-8E78-EA2F31DD4EAA}" uniqueName="int" name="int" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{DDC28D44-C5CD-4E4C-8E78-EA2F31DD4EAA}" uniqueName="int" name="int" dataDxfId="6">
       <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/Numeros/int" xmlDataType="integer"/>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C114B94E-FD69-429B-BA3C-173F0F44D3B5}" name="Tabla13" displayName="Tabla13" ref="A1:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D13" xr:uid="{CA5EA915-692C-43C8-A104-F79B1FC9DF74}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{21112DF5-1550-4674-8B93-FD7BBE514076}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{53CA23F7-FB0D-4ED6-8850-D6E56E9B1D2E}" name="PATH" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8924A21A-9011-4BA8-971B-E4CB41647895}" name="NAME" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E5720566-4A3C-4C39-A496-CB7E431EE863}" name="DESCRIPTION" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -534,11 +746,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7DA74-E98F-414F-A790-EB23CB5F8F56}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +838,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -573,7 +849,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -584,7 +860,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -595,7 +871,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -606,7 +882,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -742,6 +1018,186 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B38063-B709-46E7-89C1-B8132E9E8D45}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>123</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>180</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1">
+        <v>123</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mini Game 90% The toys change their colors when selected and go to normal if they don't match the recipe The Only thing left is make the recipe generator and connect the minigame with the metagame.
</commit_message>
<xml_diff>
--- a/Assets/Data/DataTable.xlsx
+++ b/Assets/Data/DataTable.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="13" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{448AB268-D732-44BF-9E65-64DDCE2125ED}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{F5982C64-0D13-4662-9884-5AB7F6D64AA3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,14 @@
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="file" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\Personal Projects\DataManagerTest\Assets\file.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" xr16:uid="{B0190245-DFF2-4F66-BE61-E6BF3DEC184F}" name="images" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="images" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\images.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Text</t>
   </si>
@@ -80,28 +80,52 @@
     <t>description</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>td02</t>
-  </si>
-  <si>
-    <t>Blegh</t>
-  </si>
-  <si>
-    <t>Dani</t>
-  </si>
-  <si>
-    <t>Ble</t>
-  </si>
-  <si>
-    <t>Daniela</t>
-  </si>
-  <si>
-    <t>This is a Bleg</t>
-  </si>
-  <si>
-    <t>This is a Dani</t>
+    <t>Coin</t>
+  </si>
+  <si>
+    <t>A Golden Coin</t>
+  </si>
+  <si>
+    <t>coin01</t>
+  </si>
+  <si>
+    <t>star01</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>A Golden Star</t>
+  </si>
+  <si>
+    <t>Sprites/GoldenCoin</t>
+  </si>
+  <si>
+    <t>Sprites/star</t>
+  </si>
+  <si>
+    <t>shuffle01</t>
+  </si>
+  <si>
+    <t>Sprites/shuffle</t>
+  </si>
+  <si>
+    <t>Shuffle</t>
+  </si>
+  <si>
+    <t>Shuffle Icon</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>Sprites/Circle</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>A Circle</t>
   </si>
 </sst>
 </file>
@@ -433,8 +457,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78A2D084-C518-4315-865E-394057B931C4}" name="Tabla3" displayName="Tabla3" ref="A1:D3" tableType="xml" totalsRowShown="0" connectionId="2">
-  <autoFilter ref="A1:D3" xr:uid="{B7105AD6-33EC-435A-A5D1-4F603599336D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78A2D084-C518-4315-865E-394057B931C4}" name="Tabla3" displayName="Tabla3" ref="A1:D5" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:D5" xr:uid="{B7105AD6-33EC-435A-A5D1-4F603599336D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0D8D427B-0B9C-44B0-8BCF-7D1DCDFD7373}" uniqueName="id" name="id">
       <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@id" xmlDataType="string"/>
@@ -747,14 +771,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7DA74-E98F-414F-A790-EB23CB5F8F56}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -775,30 +801,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>22</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integration with the Excel working at 20% You can succefully create Shop Items from the excel.
</commit_message>
<xml_diff>
--- a/Assets/Data/DataTable.xlsx
+++ b/Assets/Data/DataTable.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="39" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{F5982C64-0D13-4662-9884-5AB7F6D64AA3}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{3F850078-2450-44C7-BC9F-BA4ED7AD8FAD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ImagesPool" sheetId="3" r:id="rId1"/>
-    <sheet name="Images" sheetId="1" r:id="rId2"/>
+    <sheet name="MaterialsToSell" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,20 +29,29 @@
   <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="images" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\images.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="3" xr16:uid="{7AC1DD20-2D54-4E86-BDEB-23D451550935}" name="materialData" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="4" xr16:uid="{FB9D5DD2-F62A-48B1-82C9-F80717AF5DB1}" name="materialData1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="5" xr16:uid="{3C2EAF02-E5A8-45F1-88A7-6415051918DB}" name="materialData2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="6" xr16:uid="{50941153-CDA3-4302-AB69-A2D8CC62B08E}" name="materialData3" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="7" xr16:uid="{C32D347C-D15C-4B44-9CBB-2F8BA52D557D}" name="materialData4" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="8" xr16:uid="{35D2381C-D2C6-4FF1-A92C-CCBF52F3A506}" name="materialData5" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Jaime</t>
   </si>
@@ -126,13 +135,127 @@
   </si>
   <si>
     <t>A Circle</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SpriteId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>Seba</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Sprites/patito</t>
+  </si>
+  <si>
+    <t>patito</t>
+  </si>
+  <si>
+    <t>A Duck</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.016</t>
+  </si>
+  <si>
+    <t>Dani</t>
+  </si>
+  <si>
+    <t>devil</t>
+  </si>
+  <si>
+    <t>Sprites/devil</t>
+  </si>
+  <si>
+    <t>Devil</t>
+  </si>
+  <si>
+    <t>Maca</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Wii</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>Cris</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>cris</t>
+  </si>
+  <si>
+    <t>Sprites/cris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +264,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -168,107 +299,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <b val="0"/>
@@ -447,18 +491,81 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema6">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="MaterialDataList">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" name="materials" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="DataMaterial" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:attribute name="Id" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="Descripcion" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="Costo" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="SpriteId" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="R" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="G" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="B" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="A" form="unqualified" type="xsd:integer"/>
+                    </xsd:complexType>
+                  </xsd:element>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Schema ID="Schema8">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="DataList">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" nillable="true" name="materials" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Data" form="unqualified">
+                    <xsd:complexType>
+                      <xsd:attribute name="Id" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="Name" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="Price" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="Quantity" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="SpriteId" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="R" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="G" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="B" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="A" form="unqualified" type="xsd:integer"/>
+                    </xsd:complexType>
+                  </xsd:element>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="8" Name="DataList_Map" RootElement="DataList" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
+  </Map>
   <Map ID="1" Name="DataTable" RootElement="DataContainer" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="2" Name="TextureDataList_Map" RootElement="TextureDataList" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="6" Name="MaterialsToSell" RootElement="MaterialDataList" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="2" Name="SpritePool" RootElement="TextureDataList" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78A2D084-C518-4315-865E-394057B931C4}" name="Tabla3" displayName="Tabla3" ref="A1:D5" tableType="xml" totalsRowShown="0" connectionId="2">
-  <autoFilter ref="A1:D5" xr:uid="{B7105AD6-33EC-435A-A5D1-4F603599336D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78A2D084-C518-4315-865E-394057B931C4}" name="Tabla3" displayName="Tabla3" ref="A1:D8" tableType="xml" totalsRowShown="0" connectionId="2">
+  <autoFilter ref="A1:D8" xr:uid="{B7105AD6-33EC-435A-A5D1-4F603599336D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0D8D427B-0B9C-44B0-8BCF-7D1DCDFD7373}" uniqueName="id" name="id">
       <xmlColumnPr mapId="2" xpath="/TextureDataList/textures/TextureData/@id" xmlDataType="string"/>
@@ -478,17 +585,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{388CFA02-1E4E-4B7C-931A-CF3F7687FB0C}" name="Tabla1" displayName="Tabla1" ref="A1:C13" tableType="xml" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" connectionId="1">
-  <autoFilter ref="A1:C13" xr:uid="{02178007-BAB8-4248-9AC0-218326DA414F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{36992CAA-9EDF-435B-A9A8-82F8A6B3C6F5}" uniqueName="Text" name="Text" dataDxfId="8">
-      <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/@Text" xmlDataType="string"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{67386D88-482A-4804-935C-AE80D6EB4E79}" name="Tabla7" displayName="Tabla7" ref="A1:I9" tableType="xml" totalsRowShown="0" connectionId="8">
+  <autoFilter ref="A1:I9" xr:uid="{767CC81D-1787-43BE-8221-7BEFDADAF34C}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{65DD65E1-6726-4ABC-950C-AE4760CC2BCC}" uniqueName="Id" name="Id">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Id" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{597E18E7-F5C4-42C6-8840-9F56CAFAC4C6}" uniqueName="Number" name="Number" dataDxfId="7">
-      <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/@Number" xmlDataType="integer"/>
+    <tableColumn id="2" xr3:uid="{58BE4927-6A00-4E8F-9E98-B0B65EBA7B49}" uniqueName="Name" name="Name">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DDC28D44-C5CD-4E4C-8E78-EA2F31DD4EAA}" uniqueName="int" name="int" dataDxfId="6">
-      <xmlColumnPr mapId="1" xpath="/DataContainer/Items/DataItem/Numeros/int" xmlDataType="integer"/>
+    <tableColumn id="3" xr3:uid="{C239EB37-BACF-4AF4-90B4-7D0E44A66285}" uniqueName="Price" name="Price">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Price" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F678F584-971B-4610-B72C-703F7AC3A5BE}" uniqueName="Quantity" name="Quantity">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Quantity" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F4273FF9-7CE1-4D41-81E2-6C17F5A22A0B}" uniqueName="SpriteId" name="SpriteId">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@SpriteId" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{957E1188-BD4D-4384-A4C2-32B87304637A}" uniqueName="R" name="R">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@R" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B7F4C1A1-6A58-4CE4-83EA-4CEC7EF5CDBA}" uniqueName="G" name="G">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@G" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{12AE102C-CDA1-4F37-9E88-50BD8F1AEF15}" uniqueName="B" name="B">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@B" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D1CF1351-5713-49C9-B274-8C8BBB68E9E4}" uniqueName="A" name="A">
+      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@A" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -771,88 +896,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7DA74-E98F-414F-A790-EB23CB5F8F56}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -864,219 +1031,315 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D71FF8-13C4-4165-8BE8-DA08F3657EF8}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>900</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6">
+        <v>234</v>
+      </c>
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="6">
+        <v>485</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="6">
+        <v>342</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="6">
+        <v>666</v>
+      </c>
+      <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="E7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="7">
+        <v>789</v>
+      </c>
+      <c r="D8" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1097,21 +1360,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -1123,7 +1386,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1135,7 +1398,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1147,7 +1410,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -1159,7 +1422,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -1171,7 +1434,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>22</v>
@@ -1183,7 +1446,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>22</v>
@@ -1195,7 +1458,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>22</v>
@@ -1207,7 +1470,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B10" s="1">
         <v>10</v>
@@ -1219,7 +1482,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -1231,7 +1494,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
@@ -1243,7 +1506,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Hire a worker working The GUI shows correctly the workers availables to hire and how many you have working for you.
</commit_message>
<xml_diff>
--- a/Assets/Data/DataTable.xlsx
+++ b/Assets/Data/DataTable.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="161" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{3F850078-2450-44C7-BC9F-BA4ED7AD8FAD}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="23BC639085887A27961FF084604980DC82ADA257" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{27414BFB-E461-4BD2-B29F-3975E91D2CD9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ImagesPool" sheetId="3" r:id="rId1"/>
     <sheet name="MaterialsToSell" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="WorkersToHire" sheetId="5" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,13 +46,28 @@
     <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
   <connection id="8" xr16:uid="{35D2381C-D2C6-4FF1-A92C-CCBF52F3A506}" name="materialData5" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialData.xml" htmlTables="1" htmlFormat="all"/>
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialsToSell.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="9" xr16:uid="{2F007CC4-E5C9-497C-BBDF-F4EC9E3B2C75}" name="materialsToSell" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialsToSell.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="10" xr16:uid="{2EA3D753-6E3C-4786-9F9B-A1F32D9849D2}" name="materialsToSell1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\materialsToSell.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="11" xr16:uid="{1A78F0E7-C4F2-4531-8446-1CF79C943FB2}" name="workersToHire" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\workersToHire.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="12" xr16:uid="{C1B000BD-DFC6-404C-97F1-1EB20FE87FB8}" name="workersToHire1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\workersToHire.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="13" xr16:uid="{A0C73DDB-FB63-46BD-A2DE-6444F5742616}" name="workersToHire2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="E:\OneDrive\MaBoi\UTalca\Semestre 4\Taller de Videojuegos 2D\FunFactory\Assets\Data\workersToHire.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Jaime</t>
   </si>
@@ -194,9 +210,6 @@
     <t>Seba</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Sprites/patito</t>
   </si>
   <si>
@@ -206,15 +219,6 @@
     <t>A Duck</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
     <t>Dani</t>
   </si>
   <si>
@@ -242,13 +246,28 @@
     <t>Cris</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>cris</t>
   </si>
   <si>
     <t>Sprites/cris</t>
+  </si>
+  <si>
+    <t>Tired</t>
+  </si>
+  <si>
+    <t>Talent</t>
+  </si>
+  <si>
+    <t>Motivation</t>
+  </si>
+  <si>
+    <t>Worker1</t>
+  </si>
+  <si>
+    <t>DevilWorker</t>
+  </si>
+  <si>
+    <t>GoldWorker</t>
   </si>
 </sst>
 </file>
@@ -299,15 +318,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,23 +508,27 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema6">
+  <Schema ID="Schema11">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="MaterialDataList">
+      <xsd:element nillable="true" name="WorkerDataList">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" name="materials" form="unqualified">
+            <xsd:element minOccurs="0" nillable="true" name="workers" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="DataMaterial" form="unqualified">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="WorkerData" form="unqualified">
                     <xsd:complexType>
                       <xsd:attribute name="Id" form="unqualified" type="xsd:string"/>
-                      <xsd:attribute name="Descripcion" form="unqualified" type="xsd:string"/>
-                      <xsd:attribute name="Costo" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="Name" form="unqualified" type="xsd:string"/>
+                      <xsd:attribute name="Price" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="Quantity" form="unqualified" type="xsd:integer"/>
                       <xsd:attribute name="SpriteId" form="unqualified" type="xsd:string"/>
-                      <xsd:attribute name="R" form="unqualified" type="xsd:double"/>
-                      <xsd:attribute name="G" form="unqualified" type="xsd:double"/>
-                      <xsd:attribute name="B" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="Tired" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="Talent" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="Motivation" form="unqualified" type="xsd:double"/>
+                      <xsd:attribute name="R" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="G" form="unqualified" type="xsd:integer"/>
+                      <xsd:attribute name="B" form="unqualified" type="xsd:integer"/>
                       <xsd:attribute name="A" form="unqualified" type="xsd:integer"/>
                     </xsd:complexType>
                   </xsd:element>
@@ -519,15 +540,15 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema8">
+  <Schema ID="Schema13">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="DataList">
+      <xsd:element nillable="true" name="MaterialDataList">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
             <xsd:element minOccurs="0" nillable="true" name="materials" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Data" form="unqualified">
+                  <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="MaterialData" form="unqualified">
                     <xsd:complexType>
                       <xsd:attribute name="Id" form="unqualified" type="xsd:string"/>
                       <xsd:attribute name="Name" form="unqualified" type="xsd:string"/>
@@ -548,17 +569,17 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="8" Name="DataList_Map" RootElement="DataList" SchemaID="Schema8" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="8" DataBindingLoadMode="1"/>
-  </Map>
   <Map ID="1" Name="DataTable" RootElement="DataContainer" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="6" Name="MaterialsToSell" RootElement="MaterialDataList" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
+  <Map ID="13" Name="MaterialsToSell" RootElement="MaterialDataList" SchemaID="Schema13" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="10" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="2" Name="SpritePool" RootElement="TextureDataList" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="11" Name="WorkersToHire" RootElement="WorkerDataList" SchemaID="Schema11" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="13" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
@@ -585,35 +606,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{67386D88-482A-4804-935C-AE80D6EB4E79}" name="Tabla7" displayName="Tabla7" ref="A1:I9" tableType="xml" totalsRowShown="0" connectionId="8">
-  <autoFilter ref="A1:I9" xr:uid="{767CC81D-1787-43BE-8221-7BEFDADAF34C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8AEE9607-6D6B-4C79-8ABB-8932DA89210E}" name="Tabla11" displayName="Tabla11" ref="A1:I9" tableType="xml" totalsRowShown="0" connectionId="10">
+  <autoFilter ref="A1:I9" xr:uid="{5DED2345-CECF-43B8-A938-7318155AD929}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{65DD65E1-6726-4ABC-950C-AE4760CC2BCC}" uniqueName="Id" name="Id">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Id" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{58BE4927-6A00-4E8F-9E98-B0B65EBA7B49}" uniqueName="Name" name="Name">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{C239EB37-BACF-4AF4-90B4-7D0E44A66285}" uniqueName="Price" name="Price">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Price" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{F678F584-971B-4610-B72C-703F7AC3A5BE}" uniqueName="Quantity" name="Quantity">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@Quantity" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4273FF9-7CE1-4D41-81E2-6C17F5A22A0B}" uniqueName="SpriteId" name="SpriteId">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@SpriteId" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{957E1188-BD4D-4384-A4C2-32B87304637A}" uniqueName="R" name="R">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@R" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{B7F4C1A1-6A58-4CE4-83EA-4CEC7EF5CDBA}" uniqueName="G" name="G">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@G" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{12AE102C-CDA1-4F37-9E88-50BD8F1AEF15}" uniqueName="B" name="B">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@B" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{D1CF1351-5713-49C9-B274-8C8BBB68E9E4}" uniqueName="A" name="A">
-      <xmlColumnPr mapId="8" xpath="/DataList/materials/Data/@A" xmlDataType="integer"/>
+    <tableColumn id="1" xr3:uid="{DD1FB715-4F5A-4B3A-9392-6D1303FA7599}" uniqueName="Id" name="Id">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@Id" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{2CCE67E4-2037-4DE8-93EF-C4F09330AD90}" uniqueName="Name" name="Name">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{AFEAAB0F-CB62-47A6-8127-D7CD3EAEEF5D}" uniqueName="Price" name="Price">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@Price" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{D5C789D0-2581-4518-A2F6-CD430DBBE074}" uniqueName="Quantity" name="Quantity">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@Quantity" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C516523A-B84B-4B3C-81B9-D13F2B72A76D}" uniqueName="SpriteId" name="SpriteId">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@SpriteId" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{89374CCA-246B-4E3B-B367-208A5EFDD2C8}" uniqueName="R" name="R">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@R" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C301A3F0-7512-48B0-AC9E-D85253648CF1}" uniqueName="G" name="G">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@G" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C0CEAC56-1F2E-4BDB-8A2D-3A81F91C2381}" uniqueName="B" name="B">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@B" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{314BC455-D6B2-4368-8BF6-C56CFA050B40}" uniqueName="A" name="A">
+      <xmlColumnPr mapId="13" xpath="/MaterialDataList/materials/MaterialData/@A" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -621,6 +642,51 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0229F464-8E3A-44D0-A5C9-5709F78571D1}" name="Tabla9" displayName="Tabla9" ref="A1:L4" tableType="xml" totalsRowShown="0" connectionId="13">
+  <autoFilter ref="A1:L4" xr:uid="{72C7DAE4-AA87-4E4A-9584-4263988310AC}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{477B235B-6487-431A-9F69-5BB9100BB29C}" uniqueName="Id" name="Id">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Id" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C2A90144-5B8B-4474-8853-E3106AD73A26}" uniqueName="Name" name="Name">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F86642E9-0548-4B9F-9A5D-BAB80A496B3C}" uniqueName="Price" name="Price">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Price" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{7644BFF3-9687-4087-8E6E-9C22DBAD9A3C}" uniqueName="Quantity" name="Quantity">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Quantity" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{DECCFA55-5693-446F-A0F5-E1FED138C416}" uniqueName="SpriteId" name="SpriteId">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@SpriteId" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{13CD2C5D-5417-4DB7-99FA-00CFD16ACB36}" uniqueName="Tired" name="Tired">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Tired" xmlDataType="double"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{EDAB3B63-AA82-42C0-81BF-49FAE4971DCB}" uniqueName="Talent" name="Talent">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Talent" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{4DA0BDC8-360A-4833-AF09-E8C0D98501E7}" uniqueName="Motivation" name="Motivation">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@Motivation" xmlDataType="double"/>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{15E0EBEB-D7D2-4BF6-8B5E-DEBA16292EB0}" uniqueName="R" name="R">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@R" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{45367EB4-3BBC-48DB-946C-3EBA7A5EBB56}" uniqueName="G" name="G">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@G" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{F6AEF15D-AEC8-4325-9AB2-A40AB0CF6608}" uniqueName="B" name="B">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@B" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{73C3F595-3301-4404-BF8A-82D13FB28636}" uniqueName="A" name="A">
+      <xmlColumnPr mapId="11" xpath="/WorkerDataList/workers/WorkerData/@A" xmlDataType="integer"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C114B94E-FD69-429B-BA3C-173F0F44D3B5}" name="Tabla13" displayName="Tabla13" ref="A1:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D13" xr:uid="{CA5EA915-692C-43C8-A104-F79B1FC9DF74}"/>
   <tableColumns count="4">
@@ -898,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7DA74-E98F-414F-A790-EB23CB5F8F56}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -982,44 +1048,44 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1032,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D71FF8-13C4-4165-8BE8-DA08F3657EF8}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1118,7 @@
     <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -1110,23 +1176,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3">
         <v>234</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
@@ -1139,52 +1205,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4">
         <v>485</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.92</v>
+      </c>
+      <c r="H4">
+        <v>1.6E-2</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
         <v>342</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
@@ -1197,23 +1263,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
@@ -1226,23 +1292,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
         <v>666</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
@@ -1254,24 +1320,25 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
         <v>789</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
@@ -1284,24 +1351,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>51</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1313,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1321,7 +1388,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1329,7 +1396,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="E12" s="4"/>
@@ -1345,6 +1412,194 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C304D7F5-71FB-41AA-9134-56257233F138}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>8000</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>0.4</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>666</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>90</v>
+      </c>
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B38063-B709-46E7-89C1-B8132E9E8D45}">
   <dimension ref="A1:D13"/>
   <sheetViews>

</xml_diff>